<commit_message>
worked on initial data and schema
</commit_message>
<xml_diff>
--- a/Initial Data.xlsx
+++ b/Initial Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1356" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="897" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="1356" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="897" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Leader" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,11 @@
     <sheet name="User" sheetId="3" r:id="rId3"/>
     <sheet name="Ratings" sheetId="4" r:id="rId4"/>
     <sheet name="PoliticalParty" sheetId="5" r:id="rId5"/>
-    <sheet name="StateOrTerritory" sheetId="6" r:id="rId6"/>
-    <sheet name="Country" sheetId="7" r:id="rId7"/>
-    <sheet name="Region" sheetId="8" r:id="rId8"/>
-    <sheet name="Continent" sheetId="9" r:id="rId9"/>
-    <sheet name="LeaderMemberOfParty" sheetId="10" r:id="rId10"/>
+    <sheet name="LeaderMemberOfParty" sheetId="10" r:id="rId6"/>
+    <sheet name="StateOrTerritory" sheetId="6" r:id="rId7"/>
+    <sheet name="Country" sheetId="7" r:id="rId8"/>
+    <sheet name="Region" sheetId="8" r:id="rId9"/>
+    <sheet name="Continent" sheetId="9" r:id="rId10"/>
     <sheet name="CountryAlliesWith" sheetId="11" r:id="rId11"/>
     <sheet name="RegionAdjacentTo" sheetId="12" r:id="rId12"/>
     <sheet name="StateAdjacentTo" sheetId="13" r:id="rId13"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="78">
   <si>
     <t>LeaderID</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>bday</t>
-  </si>
-  <si>
-    <t>leader_name</t>
   </si>
   <si>
     <t>startdate</t>
@@ -139,9 +136,6 @@
     </r>
   </si>
   <si>
-    <t>Leader_name</t>
-  </si>
-  <si>
     <t>allied_with</t>
   </si>
   <si>
@@ -179,13 +173,139 @@
   </si>
   <si>
     <t>antarctica</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Barack</t>
+  </si>
+  <si>
+    <t>Obama</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Vladimir</t>
+  </si>
+  <si>
+    <t>Putin</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Carl XVI Gustaf</t>
+  </si>
+  <si>
+    <t>Sweeden</t>
+  </si>
+  <si>
+    <t>Tammam</t>
+  </si>
+  <si>
+    <t>Salam</t>
+  </si>
+  <si>
+    <t>Jon-Un</t>
+  </si>
+  <si>
+    <t>leader_ID</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>Position_name</t>
+  </si>
+  <si>
+    <t>Supreme Leader</t>
+  </si>
+  <si>
+    <t>President</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>sweeden</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>finiteZ</t>
+  </si>
+  <si>
+    <t>hamiltjc@rose-hulman.edu</t>
+  </si>
+  <si>
+    <t>bonattt</t>
+  </si>
+  <si>
+    <t>bonattt@rose-hulman.edu</t>
+  </si>
+  <si>
+    <t>fineral</t>
+  </si>
+  <si>
+    <t>fineral@rose-hulman.edu</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>illinois</t>
+  </si>
+  <si>
+    <t>countryID</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>lebenon</t>
+  </si>
+  <si>
+    <t>Acting President</t>
+  </si>
+  <si>
+    <t>republican party of America</t>
+  </si>
+  <si>
+    <t>democrat party of America</t>
+  </si>
+  <si>
+    <t>Leader_ID</t>
+  </si>
+  <si>
+    <t>party_ID</t>
+  </si>
+  <si>
+    <t>continentID</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>midwest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +338,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -236,10 +364,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -247,8 +376,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -551,13 +684,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -579,6 +715,76 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -587,29 +793,80 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>24</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
         <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -634,10 +891,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -661,10 +918,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -688,10 +945,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -701,31 +958,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>39833</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>41036</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>40888</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>26922</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>41685</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -735,37 +1081,67 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="D2" s="3"/>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -775,7 +1151,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,16 +1161,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -804,23 +1180,39 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -830,10 +1222,56 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,13 +1283,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -859,26 +1330,104 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -886,11 +1435,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -899,104 +1448,39 @@
     <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>